<commit_message>
ProductCodes and DeliveryDate added
</commit_message>
<xml_diff>
--- a/output/products.xlsx
+++ b/output/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubin\PycharmProjects\Charcoal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741122E-025C-4E07-95FF-E340B09CE947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3755752B-E72B-4698-BF2A-FBF83C6E5EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0DD7FB95-636C-47AB-B62C-6E220D87849D}"/>
+    <workbookView xWindow="2988" yWindow="2076" windowWidth="17280" windowHeight="10644" xr2:uid="{0DD7FB95-636C-47AB-B62C-6E220D87849D}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,27 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Уголь древесно-брикетный (евроуголь) 10 кг</t>
-  </si>
-  <si>
-    <t>Уголь брикетный 10 кг в коробке</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Наличный расчет</t>
   </si>
@@ -54,25 +39,61 @@
     <t>Наименование</t>
   </si>
   <si>
-    <t>Уголь древесный 10 л</t>
-  </si>
-  <si>
-    <t>Уголь древесный 20 л</t>
-  </si>
-  <si>
-    <t>Уголь березовый 10 литров</t>
-  </si>
-  <si>
-    <t>Уголь березовый 20 литров</t>
-  </si>
-  <si>
     <t>Уголь березовый 10 литров (эконом)</t>
   </si>
   <si>
-    <t>Древесно-угольный микс 3кг</t>
-  </si>
-  <si>
-    <t>Уголь березовый 50л (10кг)</t>
+    <t>Уголь березовый 50л (10кг.)</t>
+  </si>
+  <si>
+    <t>Уголь древесный 10 л.</t>
+  </si>
+  <si>
+    <t>Уголь древесный 20 л.</t>
+  </si>
+  <si>
+    <t>Уголь брикетный 10 кг. в коробке</t>
+  </si>
+  <si>
+    <t>Уголь древесно-брикетный (евроуголь) 10 кг.</t>
+  </si>
+  <si>
+    <t>Код</t>
+  </si>
+  <si>
+    <t>Древесно-угольный  "MiX" 3кг.</t>
+  </si>
+  <si>
+    <t>Уголь "Берёзовый" ХТС 10 литров</t>
+  </si>
+  <si>
+    <t>Уголь "Берёзовый" ХТС 20 литров</t>
+  </si>
+  <si>
+    <t>50л</t>
+  </si>
+  <si>
+    <t>к1с</t>
+  </si>
+  <si>
+    <t>к2с</t>
+  </si>
+  <si>
+    <t>3м</t>
+  </si>
+  <si>
+    <t>10б</t>
+  </si>
+  <si>
+    <t>20б</t>
+  </si>
+  <si>
+    <t>д10</t>
+  </si>
+  <si>
+    <t>д20</t>
+  </si>
+  <si>
+    <t>к10б</t>
   </si>
 </sst>
 </file>
@@ -432,158 +453,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04470D0A-96E8-4546-B70B-DC713573B028}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="1">
+        <v>500</v>
+      </c>
+      <c r="D2" s="1">
+        <v>550</v>
+      </c>
+      <c r="E2" s="1">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1">
+        <v>550</v>
+      </c>
+      <c r="E3" s="1">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>450</v>
+      </c>
+      <c r="D4" s="1">
+        <v>495</v>
+      </c>
+      <c r="E4" s="1">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>200</v>
+      </c>
+      <c r="D5" s="1">
+        <v>220</v>
+      </c>
+      <c r="E5" s="1">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>130</v>
+      </c>
+      <c r="D6" s="1">
+        <v>143</v>
+      </c>
+      <c r="E6" s="1">
+        <v>175.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>260</v>
+      </c>
+      <c r="D7" s="1">
+        <v>286</v>
+      </c>
+      <c r="E7" s="1">
+        <v>343.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1">
+        <v>60</v>
+      </c>
+      <c r="E8" s="1">
+        <v>72.599999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>110</v>
+      </c>
+      <c r="D9" s="1">
+        <v>120</v>
+      </c>
+      <c r="E9" s="1">
+        <v>145.19999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1">
-        <v>130</v>
-      </c>
-      <c r="C2" s="1">
-        <v>143</v>
-      </c>
-      <c r="D2" s="1">
-        <v>175.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>260</v>
-      </c>
-      <c r="C3" s="1">
-        <v>286</v>
-      </c>
-      <c r="D3" s="1">
-        <v>343.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1">
-        <v>500</v>
-      </c>
-      <c r="C4" s="1">
-        <v>550</v>
-      </c>
-      <c r="D4" s="1">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="C10" s="1">
         <v>120</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D10" s="1">
         <v>132</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E10" s="1">
         <v>160.80000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <v>200</v>
-      </c>
-      <c r="C6" s="1">
-        <v>220</v>
-      </c>
-      <c r="D6" s="1">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>55</v>
-      </c>
-      <c r="C7" s="1">
-        <v>60.5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>72.599999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>110</v>
-      </c>
-      <c r="C8" s="1">
-        <v>121</v>
-      </c>
-      <c r="D8" s="1">
-        <v>145.19999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>500</v>
-      </c>
-      <c r="C9" s="1">
-        <v>550</v>
-      </c>
-      <c r="D9" s="1">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1">
-        <v>450</v>
-      </c>
-      <c r="C10" s="1">
-        <v>495</v>
-      </c>
-      <c r="D10" s="1">
-        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>